<commit_message>
more progress on new weapon modding code, pending testing
</commit_message>
<xml_diff>
--- a/5_weapon_database/weapon_database.xlsx
+++ b/5_weapon_database/weapon_database.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="101">
   <si>
     <t>name</t>
   </si>
@@ -91,6 +91,9 @@
     <t>tetra</t>
   </si>
   <si>
+    <t>lenz</t>
+  </si>
+  <si>
     <t>mastery</t>
   </si>
   <si>
@@ -109,16 +112,25 @@
     <t>rifle</t>
   </si>
   <si>
+    <t>bow</t>
+  </si>
+  <si>
     <t>trigger</t>
   </si>
   <si>
     <t>auto</t>
   </si>
   <si>
+    <t>charge</t>
+  </si>
+  <si>
     <t>ammo_type</t>
   </si>
   <si>
     <t>FR</t>
+  </si>
+  <si>
+    <t>charge_time</t>
   </si>
   <si>
     <t>MAG</t>
@@ -346,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -354,6 +366,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -655,10 +670,10 @@
       <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
       <c r="Y1" s="2" t="s">
@@ -670,10 +685,13 @@
       <c r="AA1" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="AB1" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2">
         <v>13.0</v>
@@ -741,7 +759,7 @@
       <c r="W2" s="2">
         <v>7.0</v>
       </c>
-      <c r="X2" s="3">
+      <c r="X2" s="2">
         <v>14.0</v>
       </c>
       <c r="Y2" s="2">
@@ -750,345 +768,360 @@
       <c r="Z2" s="2">
         <v>3.0</v>
       </c>
-      <c r="AA2" s="3">
+      <c r="AA2" s="2">
         <v>4.0</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>8.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="AA5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AA6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B7" s="2">
         <v>2.5</v>
@@ -1153,982 +1186,1019 @@
       <c r="V7" s="2">
         <v>3.0</v>
       </c>
-      <c r="W7" s="3">
+      <c r="W7" s="2">
         <v>2.0</v>
       </c>
-      <c r="X7" s="3">
+      <c r="X7" s="2">
         <v>3.67</v>
       </c>
-      <c r="Y7" s="3">
+      <c r="Y7" s="2">
         <v>2.0</v>
       </c>
       <c r="Z7" s="2">
         <v>6.67</v>
       </c>
-      <c r="AA7" s="3">
+      <c r="AA7" s="2">
         <v>7.08</v>
       </c>
+      <c r="AB7" s="2">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="2">
-        <v>7.0</v>
-      </c>
-      <c r="C8" s="2">
-        <v>40.0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>60.0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>60.0</v>
-      </c>
-      <c r="F8" s="2">
-        <v>60.0</v>
-      </c>
-      <c r="G8" s="2">
-        <v>90.0</v>
-      </c>
-      <c r="H8" s="2">
-        <v>45.0</v>
-      </c>
-      <c r="I8" s="2">
-        <v>60.0</v>
-      </c>
-      <c r="J8" s="2">
-        <v>75.0</v>
-      </c>
-      <c r="K8" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="L8" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="M8" s="2">
-        <v>45.0</v>
-      </c>
-      <c r="N8" s="2">
-        <v>60.0</v>
-      </c>
-      <c r="O8" s="2">
-        <v>60.0</v>
-      </c>
-      <c r="P8" s="2">
-        <v>120.0</v>
-      </c>
-      <c r="Q8" s="2">
-        <v>30.0</v>
-      </c>
-      <c r="R8" s="2">
-        <v>60.0</v>
-      </c>
-      <c r="S8" s="2">
-        <v>70.0</v>
-      </c>
-      <c r="T8" s="2">
-        <v>60.0</v>
-      </c>
-      <c r="U8" s="2">
-        <v>60.0</v>
-      </c>
-      <c r="V8" s="2">
-        <v>60.0</v>
-      </c>
-      <c r="W8" s="2">
-        <v>60.0</v>
-      </c>
-      <c r="X8" s="3">
-        <v>80.0</v>
-      </c>
-      <c r="Y8" s="2">
-        <v>80.0</v>
-      </c>
-      <c r="Z8" s="2">
-        <v>60.0</v>
-      </c>
-      <c r="AA8" s="2">
-        <v>60.0</v>
+      <c r="A8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="O8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="P8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="R8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="S8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="T8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="U8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="V8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="W8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="X8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="Y8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="Z8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="AA8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="AB8" s="4">
+        <v>0.6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="4">
-        <v>1.0E9</v>
+        <v>40</v>
+      </c>
+      <c r="B9" s="2">
+        <v>7.0</v>
       </c>
       <c r="C9" s="2">
-        <v>800.0</v>
+        <v>40.0</v>
       </c>
       <c r="D9" s="2">
-        <v>840.0</v>
+        <v>60.0</v>
       </c>
       <c r="E9" s="2">
-        <v>540.0</v>
+        <v>60.0</v>
       </c>
       <c r="F9" s="2">
-        <v>540.0</v>
+        <v>60.0</v>
       </c>
       <c r="G9" s="2">
-        <v>540.0</v>
+        <v>90.0</v>
       </c>
       <c r="H9" s="2">
-        <v>540.0</v>
+        <v>45.0</v>
       </c>
       <c r="I9" s="2">
-        <v>540.0</v>
+        <v>60.0</v>
       </c>
       <c r="J9" s="2">
-        <v>600.0</v>
+        <v>75.0</v>
       </c>
       <c r="K9" s="2">
-        <v>550.0</v>
+        <v>50.0</v>
       </c>
       <c r="L9" s="2">
-        <v>540.0</v>
+        <v>50.0</v>
       </c>
       <c r="M9" s="2">
-        <v>540.0</v>
+        <v>45.0</v>
       </c>
       <c r="N9" s="2">
-        <v>540.0</v>
+        <v>60.0</v>
       </c>
       <c r="O9" s="2">
-        <v>750.0</v>
+        <v>60.0</v>
       </c>
       <c r="P9" s="2">
-        <v>1000.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q9" s="2">
-        <v>540.0</v>
+        <v>30.0</v>
       </c>
       <c r="R9" s="2">
-        <v>540.0</v>
+        <v>60.0</v>
       </c>
       <c r="S9" s="2">
-        <v>540.0</v>
+        <v>70.0</v>
       </c>
       <c r="T9" s="2">
-        <v>540.0</v>
+        <v>60.0</v>
       </c>
       <c r="U9" s="2">
-        <v>540.0</v>
+        <v>60.0</v>
       </c>
       <c r="V9" s="2">
-        <v>540.0</v>
+        <v>60.0</v>
       </c>
       <c r="W9" s="2">
-        <v>540.0</v>
-      </c>
-      <c r="X9" s="3">
-        <v>320.0</v>
+        <v>60.0</v>
+      </c>
+      <c r="X9" s="2">
+        <v>80.0</v>
       </c>
       <c r="Y9" s="2">
-        <v>320.0</v>
+        <v>80.0</v>
       </c>
       <c r="Z9" s="2">
-        <v>54.0</v>
+        <v>60.0</v>
       </c>
       <c r="AA9" s="2">
-        <v>54.0</v>
+        <v>60.0</v>
+      </c>
+      <c r="AB9" s="2">
+        <v>1.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1.0</v>
+        <v>41</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1.0E9</v>
       </c>
       <c r="C10" s="2">
-        <v>1.0</v>
+        <v>800.0</v>
       </c>
       <c r="D10" s="2">
-        <v>1.0</v>
+        <v>840.0</v>
       </c>
       <c r="E10" s="2">
-        <v>1.0</v>
+        <v>540.0</v>
       </c>
       <c r="F10" s="2">
-        <v>1.0</v>
+        <v>540.0</v>
       </c>
       <c r="G10" s="2">
-        <v>1.0</v>
+        <v>540.0</v>
       </c>
       <c r="H10" s="2">
-        <v>1.0</v>
+        <v>540.0</v>
       </c>
       <c r="I10" s="2">
-        <v>1.0</v>
+        <v>540.0</v>
       </c>
       <c r="J10" s="2">
-        <v>1.0</v>
+        <v>600.0</v>
       </c>
       <c r="K10" s="2">
-        <v>1.0</v>
+        <v>550.0</v>
       </c>
       <c r="L10" s="2">
-        <v>1.0</v>
+        <v>540.0</v>
       </c>
       <c r="M10" s="2">
-        <v>1.0</v>
+        <v>540.0</v>
       </c>
       <c r="N10" s="2">
-        <v>1.0</v>
+        <v>540.0</v>
       </c>
       <c r="O10" s="2">
-        <v>1.0</v>
+        <v>750.0</v>
       </c>
       <c r="P10" s="2">
-        <v>1.0</v>
+        <v>1000.0</v>
       </c>
       <c r="Q10" s="2">
-        <v>1.0</v>
+        <v>540.0</v>
       </c>
       <c r="R10" s="2">
-        <v>1.0</v>
+        <v>540.0</v>
       </c>
       <c r="S10" s="2">
-        <v>1.0</v>
+        <v>540.0</v>
       </c>
       <c r="T10" s="2">
-        <v>1.0</v>
+        <v>540.0</v>
       </c>
       <c r="U10" s="2">
-        <v>5.0</v>
-      </c>
-      <c r="V10" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="W10" s="3">
-        <v>1.0</v>
+        <v>540.0</v>
+      </c>
+      <c r="V10" s="2">
+        <v>540.0</v>
+      </c>
+      <c r="W10" s="2">
+        <v>540.0</v>
       </c>
       <c r="X10" s="2">
-        <v>2.0</v>
-      </c>
-      <c r="Y10" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="Z10" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="AA10" s="2">
-        <v>1.0</v>
+        <v>320.0</v>
+      </c>
+      <c r="Y10" s="2">
+        <v>320.0</v>
+      </c>
+      <c r="Z10" s="4">
+        <v>540.0</v>
+      </c>
+      <c r="AA10" s="4">
+        <v>540.0</v>
+      </c>
+      <c r="AB10" s="2">
+        <v>6.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B11" s="2">
-        <v>1.25</v>
+        <v>1.0</v>
       </c>
       <c r="C11" s="2">
-        <v>1.4</v>
+        <v>1.0</v>
       </c>
       <c r="D11" s="2">
-        <v>1.1</v>
+        <v>1.0</v>
       </c>
       <c r="E11" s="2">
-        <v>2.6</v>
+        <v>1.0</v>
       </c>
       <c r="F11" s="2">
-        <v>2.4</v>
+        <v>1.0</v>
       </c>
       <c r="G11" s="2">
-        <v>2.4</v>
+        <v>1.0</v>
       </c>
       <c r="H11" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="I11" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="J11" s="2">
-        <v>2.15</v>
+        <v>1.0</v>
       </c>
       <c r="K11" s="2">
-        <v>1.75</v>
+        <v>1.0</v>
       </c>
       <c r="L11" s="2">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="M11" s="2">
-        <v>1.8</v>
+        <v>1.0</v>
       </c>
       <c r="N11" s="2">
-        <v>1.8</v>
+        <v>1.0</v>
       </c>
       <c r="O11" s="2">
-        <v>2.4</v>
+        <v>1.0</v>
       </c>
       <c r="P11" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="Q11" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="R11" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="S11" s="2">
-        <v>1.7</v>
+        <v>1.0</v>
       </c>
       <c r="T11" s="2">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="U11" s="2">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="V11" s="2">
         <v>2.0</v>
       </c>
       <c r="W11" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="X11" s="2">
         <v>2.0</v>
       </c>
-      <c r="X11" s="3">
-        <v>2.4</v>
-      </c>
       <c r="Y11" s="2">
-        <v>2.4</v>
+        <v>1.0</v>
       </c>
       <c r="Z11" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="AA11" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="AB11" s="2">
+        <v>1.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="5">
-        <f t="shared" ref="B12:AA12" si="1">1/B11</f>
+        <v>43</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1.1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="F12" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="G12" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="H12" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="I12" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="J12" s="2">
+        <v>2.15</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="L12" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="M12" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="N12" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="O12" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="P12" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="R12" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="S12" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="T12" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="U12" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="V12" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="W12" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="X12" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="Y12" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="Z12" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="AA12" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="AB12" s="2">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="6">
+        <f t="shared" ref="B13:AB13" si="1">1/B12</f>
         <v>0.8</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C13" s="6">
         <f t="shared" si="1"/>
         <v>0.7142857143</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D13" s="6">
         <f t="shared" si="1"/>
         <v>0.9090909091</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E13" s="6">
         <f t="shared" si="1"/>
         <v>0.3846153846</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F13" s="6">
         <f t="shared" si="1"/>
         <v>0.4166666667</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G13" s="6">
         <f t="shared" si="1"/>
         <v>0.4166666667</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H13" s="6">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I13" s="6">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J13" s="6">
         <f t="shared" si="1"/>
         <v>0.4651162791</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K13" s="6">
         <f t="shared" si="1"/>
         <v>0.5714285714</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L13" s="6">
         <f t="shared" si="1"/>
         <v>0.3333333333</v>
       </c>
-      <c r="M12" s="5">
+      <c r="M13" s="6">
         <f t="shared" si="1"/>
         <v>0.5555555556</v>
       </c>
-      <c r="N12" s="5">
+      <c r="N13" s="6">
         <f t="shared" si="1"/>
         <v>0.5555555556</v>
       </c>
-      <c r="O12" s="5">
+      <c r="O13" s="6">
         <f t="shared" si="1"/>
         <v>0.4166666667</v>
       </c>
-      <c r="P12" s="5">
+      <c r="P13" s="6">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="Q12" s="5">
+      <c r="Q13" s="6">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="R12" s="5">
+      <c r="R13" s="6">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="S12" s="5">
+      <c r="S13" s="6">
         <f t="shared" si="1"/>
         <v>0.5882352941</v>
       </c>
-      <c r="T12" s="5">
+      <c r="T13" s="6">
         <f t="shared" si="1"/>
         <v>0.3333333333</v>
       </c>
-      <c r="U12" s="5">
+      <c r="U13" s="6">
         <f t="shared" si="1"/>
         <v>0.3333333333</v>
       </c>
-      <c r="V12" s="5">
+      <c r="V13" s="6">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="W12" s="5">
+      <c r="W13" s="6">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="X12" s="5">
+      <c r="X13" s="6">
         <f t="shared" si="1"/>
         <v>0.4166666667</v>
       </c>
-      <c r="Y12" s="5">
+      <c r="Y13" s="6">
         <f t="shared" si="1"/>
         <v>0.4166666667</v>
       </c>
-      <c r="Z12" s="5">
+      <c r="Z13" s="6">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="AA12" s="5">
+      <c r="AA13" s="6">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="2">
-        <v>0.85</v>
-      </c>
-      <c r="C13" s="2">
-        <v>1.05</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0.95</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1.25</v>
-      </c>
-      <c r="F13" s="2">
-        <v>1.15</v>
-      </c>
-      <c r="G13" s="2">
-        <v>1.15</v>
-      </c>
-      <c r="H13" s="2">
-        <v>1.35</v>
-      </c>
-      <c r="I13" s="2">
-        <v>1.35</v>
-      </c>
-      <c r="J13" s="2">
-        <v>1.25</v>
-      </c>
-      <c r="K13" s="2">
-        <v>1.3</v>
-      </c>
-      <c r="L13" s="2">
-        <v>1.45</v>
-      </c>
-      <c r="M13" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="N13" s="2">
-        <v>1.35</v>
-      </c>
-      <c r="O13" s="2">
-        <v>1.35</v>
-      </c>
-      <c r="P13" s="2">
-        <v>1.3</v>
-      </c>
-      <c r="Q13" s="2">
-        <v>1.35</v>
-      </c>
-      <c r="R13" s="2">
-        <v>1.28</v>
-      </c>
-      <c r="S13" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="T13" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="U13" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="V13" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="W13" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="X13" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="Y13" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="Z13" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="AA13" s="3">
-        <v>1.45</v>
+      <c r="AB13" s="6">
+        <f t="shared" si="1"/>
+        <v>1.666666667</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B14" s="2">
-        <v>1.0</v>
+        <v>0.85</v>
       </c>
       <c r="C14" s="2">
-        <v>1.0</v>
+        <v>1.05</v>
       </c>
       <c r="D14" s="2">
-        <v>1.0</v>
+        <v>0.95</v>
       </c>
       <c r="E14" s="2">
-        <v>1.0</v>
+        <v>1.25</v>
       </c>
       <c r="F14" s="2">
-        <v>1.0</v>
+        <v>1.15</v>
       </c>
       <c r="G14" s="2">
-        <v>1.0</v>
+        <v>1.15</v>
       </c>
       <c r="H14" s="2">
-        <v>1.0</v>
+        <v>1.35</v>
       </c>
       <c r="I14" s="2">
-        <v>1.0</v>
+        <v>1.35</v>
       </c>
       <c r="J14" s="2">
-        <v>1.0</v>
+        <v>1.25</v>
       </c>
       <c r="K14" s="2">
-        <v>1.0</v>
+        <v>1.3</v>
       </c>
       <c r="L14" s="2">
-        <v>1.0</v>
+        <v>1.45</v>
       </c>
       <c r="M14" s="2">
-        <v>1.0</v>
+        <v>1.4</v>
       </c>
       <c r="N14" s="2">
-        <v>1.0</v>
+        <v>1.35</v>
       </c>
       <c r="O14" s="2">
-        <v>1.0</v>
+        <v>1.35</v>
       </c>
       <c r="P14" s="2">
-        <v>1.0</v>
+        <v>1.3</v>
       </c>
       <c r="Q14" s="2">
-        <v>1.0</v>
+        <v>1.35</v>
       </c>
       <c r="R14" s="2">
-        <v>1.0</v>
+        <v>1.28</v>
       </c>
       <c r="S14" s="2">
         <v>1.0</v>
       </c>
       <c r="T14" s="2">
-        <v>1.0</v>
+        <v>1.5</v>
       </c>
       <c r="U14" s="2">
-        <v>1.0</v>
+        <v>1.5</v>
       </c>
       <c r="V14" s="2">
-        <v>1.0</v>
+        <v>1.4</v>
       </c>
       <c r="W14" s="2">
-        <v>1.0</v>
+        <v>1.4</v>
       </c>
       <c r="X14" s="2">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="Y14" s="2">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="Z14" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="AA14" s="2">
-        <v>1.0</v>
+        <v>1.5</v>
+      </c>
+      <c r="AA14" s="4">
+        <v>1.45</v>
+      </c>
+      <c r="AB14" s="2">
+        <v>0.95</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="6" t="s">
-        <v>43</v>
+      <c r="A15" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="B15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="I15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="M15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="N15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="P15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="R15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="S15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="T15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="U15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="V15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="W15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="X15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="Z15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="AA15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="AB15" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="2">
         <v>0.25</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C16" s="2">
         <v>0.26</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D16" s="2">
         <v>0.28</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E16" s="2">
         <v>0.1</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F16" s="2">
         <v>0.12</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G16" s="2">
         <v>0.3</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H16" s="2">
         <v>0.12</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I16" s="2">
         <v>0.08</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J16" s="2">
         <v>0.12</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K16" s="2">
         <v>0.16</v>
       </c>
-      <c r="L15" s="2">
+      <c r="L16" s="2">
         <v>0.23</v>
       </c>
-      <c r="M15" s="2">
+      <c r="M16" s="2">
         <v>0.08</v>
       </c>
-      <c r="N15" s="2">
+      <c r="N16" s="2">
         <v>0.08</v>
       </c>
-      <c r="O15" s="2">
+      <c r="O16" s="2">
         <v>0.25</v>
       </c>
-      <c r="P15" s="2">
+      <c r="P16" s="2">
         <v>0.25</v>
       </c>
-      <c r="Q15" s="2">
+      <c r="Q16" s="2">
         <v>0.09</v>
       </c>
-      <c r="R15" s="2">
+      <c r="R16" s="2">
         <v>0.13</v>
       </c>
-      <c r="S15" s="2">
+      <c r="S16" s="2">
         <v>0.23</v>
       </c>
-      <c r="T15" s="2">
+      <c r="T16" s="2">
         <v>0.025</v>
       </c>
-      <c r="U15" s="3">
+      <c r="U16" s="2">
         <v>0.025</v>
       </c>
-      <c r="V15" s="2">
+      <c r="V16" s="2">
         <v>0.12</v>
       </c>
-      <c r="W15" s="3">
+      <c r="W16" s="2">
         <v>0.25</v>
       </c>
-      <c r="X15" s="3">
+      <c r="X16" s="2">
         <v>0.18</v>
       </c>
-      <c r="Y15" s="3">
+      <c r="Y16" s="2">
         <v>0.26</v>
       </c>
-      <c r="Z15" s="2">
+      <c r="Z16" s="2">
         <v>0.04</v>
       </c>
-      <c r="AA15" s="3">
+      <c r="AA16" s="2">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="2">
+      <c r="AB16" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="2">
         <v>2.1</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C17" s="2">
         <v>3.0</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D17" s="2">
         <v>3.0</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E17" s="2">
         <v>1.8</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F17" s="2">
         <v>2.0</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G17" s="2">
         <v>2.4</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H17" s="2">
         <v>1.6</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I17" s="2">
         <v>1.5</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J17" s="2">
         <v>2.0</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K17" s="2">
         <v>2.0</v>
       </c>
-      <c r="L16" s="2">
+      <c r="L17" s="2">
         <v>2.5</v>
       </c>
-      <c r="M16" s="2">
+      <c r="M17" s="2">
         <v>1.6</v>
       </c>
-      <c r="N16" s="2">
+      <c r="N17" s="2">
         <v>2.0</v>
       </c>
-      <c r="O16" s="2">
+      <c r="O17" s="2">
         <v>2.0</v>
       </c>
-      <c r="P16" s="2">
+      <c r="P17" s="2">
         <v>2.5</v>
       </c>
-      <c r="Q16" s="2">
+      <c r="Q17" s="2">
         <v>1.5</v>
       </c>
-      <c r="R16" s="2">
+      <c r="R17" s="2">
         <v>2.0</v>
       </c>
-      <c r="S16" s="2">
+      <c r="S17" s="2">
         <v>2.1</v>
       </c>
-      <c r="T16" s="2">
+      <c r="T17" s="2">
         <v>1.5</v>
       </c>
-      <c r="U16" s="2">
+      <c r="U17" s="2">
         <v>1.5</v>
       </c>
-      <c r="V16" s="2">
+      <c r="V17" s="2">
         <v>2.0</v>
       </c>
-      <c r="W16" s="2">
+      <c r="W17" s="2">
         <v>2.0</v>
       </c>
-      <c r="X16" s="2">
+      <c r="X17" s="2">
         <v>2.0</v>
       </c>
-      <c r="Y16" s="2">
+      <c r="Y17" s="2">
         <v>2.0</v>
       </c>
-      <c r="Z16" s="2">
+      <c r="Z17" s="2">
         <v>1.5</v>
       </c>
-      <c r="AA16" s="3">
+      <c r="AA17" s="2">
         <v>2.0</v>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="2">
+      <c r="AB17" s="2">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="2">
         <v>0.23</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C18" s="2">
         <v>0.1</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D18" s="2">
         <v>0.14</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E18" s="2">
         <v>0.14</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F18" s="2">
         <v>0.34</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G18" s="2">
         <v>0.16</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H18" s="2">
         <v>0.06</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I18" s="2">
         <v>0.05</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J18" s="2">
         <v>0.26</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K18" s="2">
         <v>0.16</v>
       </c>
-      <c r="L17" s="2">
+      <c r="L18" s="2">
         <v>0.21</v>
       </c>
-      <c r="M17" s="2">
+      <c r="M18" s="2">
         <v>0.22</v>
       </c>
-      <c r="N17" s="2">
+      <c r="N18" s="2">
         <v>0.3</v>
       </c>
-      <c r="O17" s="2">
+      <c r="O18" s="2">
         <v>0.2</v>
       </c>
-      <c r="P17" s="2">
+      <c r="P18" s="2">
         <v>0.21</v>
       </c>
-      <c r="Q17" s="2">
+      <c r="Q18" s="2">
         <v>0.15</v>
       </c>
-      <c r="R17" s="2">
+      <c r="R18" s="2">
         <v>0.25</v>
       </c>
-      <c r="S17" s="2">
+      <c r="S18" s="2">
         <v>0.31</v>
       </c>
-      <c r="T17" s="2">
+      <c r="T18" s="2">
         <v>0.15</v>
       </c>
-      <c r="U17" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="V17" s="2">
+      <c r="U18" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="V18" s="2">
         <v>0.24</v>
       </c>
-      <c r="W17" s="3">
+      <c r="W18" s="2">
         <v>0.35</v>
       </c>
-      <c r="X17" s="3">
+      <c r="X18" s="2">
         <v>0.3</v>
       </c>
-      <c r="Y17" s="3">
+      <c r="Y18" s="2">
         <v>0.38</v>
       </c>
-      <c r="Z17" s="2">
+      <c r="Z18" s="2">
         <v>0.2</v>
       </c>
-      <c r="AA17" s="3">
+      <c r="AA18" s="2">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C18" s="2">
+      <c r="AB18" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C19" s="2">
         <v>5.8</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D19" s="2">
         <v>5.8</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E19" s="2">
         <v>2.5</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F19" s="2">
         <v>4.6</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G19" s="2">
         <v>3.0</v>
-      </c>
-      <c r="H18" s="2">
-        <v>7.9</v>
-      </c>
-      <c r="I18" s="2">
-        <v>4.5</v>
-      </c>
-      <c r="J18" s="2">
-        <v>1.75</v>
-      </c>
-      <c r="K18" s="2">
-        <v>12.25</v>
-      </c>
-      <c r="L18" s="2">
-        <v>30.0</v>
-      </c>
-      <c r="M18" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="N18" s="2">
-        <v>6.4</v>
-      </c>
-      <c r="O18" s="2">
-        <v>4.4</v>
-      </c>
-      <c r="P18" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="Q18" s="2">
-        <v>13.0</v>
-      </c>
-      <c r="R18" s="2">
-        <v>14.1</v>
-      </c>
-      <c r="S18" s="2">
-        <v>7.1</v>
-      </c>
-      <c r="T18" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="U18" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="V18" s="2">
-        <v>20.0</v>
-      </c>
-      <c r="W18" s="3">
-        <v>10.0</v>
-      </c>
-      <c r="X18" s="2">
-        <v>20.0</v>
-      </c>
-      <c r="Y18" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="Z18" s="2">
-        <v>6.4</v>
-      </c>
-      <c r="AA18" s="3">
-        <v>7.6</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C19" s="2">
-        <v>6.7</v>
-      </c>
-      <c r="D19" s="2">
-        <v>6.7</v>
-      </c>
-      <c r="E19" s="2">
-        <v>20.0</v>
-      </c>
-      <c r="F19" s="2">
-        <v>41.4</v>
-      </c>
-      <c r="G19" s="2">
-        <v>27.0</v>
       </c>
       <c r="H19" s="2">
         <v>7.9</v>
@@ -2137,229 +2207,238 @@
         <v>4.5</v>
       </c>
       <c r="J19" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="K19" s="2">
         <v>12.25</v>
       </c>
-      <c r="K19" s="2">
-        <v>1.75</v>
-      </c>
       <c r="L19" s="2">
-        <v>24.0</v>
+        <v>30.0</v>
       </c>
       <c r="M19" s="2">
-        <v>22.5</v>
+        <v>6.0</v>
       </c>
       <c r="N19" s="2">
-        <v>24.0</v>
+        <v>6.4</v>
       </c>
       <c r="O19" s="2">
-        <v>3.7</v>
+        <v>4.4</v>
       </c>
       <c r="P19" s="2">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="Q19" s="2">
-        <v>8.7</v>
+        <v>13.0</v>
       </c>
       <c r="R19" s="2">
-        <v>9.3</v>
+        <v>14.1</v>
       </c>
       <c r="S19" s="2">
-        <v>6.2</v>
+        <v>7.1</v>
       </c>
       <c r="T19" s="2">
-        <v>15.0</v>
+        <v>2.5</v>
       </c>
       <c r="U19" s="2">
         <v>0.0</v>
       </c>
       <c r="V19" s="2">
-        <v>10.0</v>
+        <v>20.0</v>
       </c>
       <c r="W19" s="2">
         <v>10.0</v>
       </c>
       <c r="X19" s="2">
+        <v>20.0</v>
+      </c>
+      <c r="Y19" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Z19" s="2">
+        <v>6.4</v>
+      </c>
+      <c r="AA19" s="2">
+        <v>7.6</v>
+      </c>
+      <c r="AB19" s="2">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C20" s="2">
+        <v>6.7</v>
+      </c>
+      <c r="D20" s="2">
+        <v>6.7</v>
+      </c>
+      <c r="E20" s="2">
+        <v>20.0</v>
+      </c>
+      <c r="F20" s="2">
+        <v>41.4</v>
+      </c>
+      <c r="G20" s="2">
+        <v>27.0</v>
+      </c>
+      <c r="H20" s="2">
+        <v>7.9</v>
+      </c>
+      <c r="I20" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="J20" s="2">
+        <v>12.25</v>
+      </c>
+      <c r="K20" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="L20" s="2">
+        <v>24.0</v>
+      </c>
+      <c r="M20" s="2">
+        <v>22.5</v>
+      </c>
+      <c r="N20" s="2">
+        <v>24.0</v>
+      </c>
+      <c r="O20" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="P20" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>8.7</v>
+      </c>
+      <c r="R20" s="2">
+        <v>9.3</v>
+      </c>
+      <c r="S20" s="2">
+        <v>6.2</v>
+      </c>
+      <c r="T20" s="2">
+        <v>15.0</v>
+      </c>
+      <c r="U20" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="V20" s="2">
         <v>10.0</v>
       </c>
-      <c r="Y19" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="Z19" s="2">
+      <c r="W20" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="X20" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="Y20" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Z20" s="2">
         <v>25.6</v>
       </c>
-      <c r="AA19" s="3">
+      <c r="AA20" s="2">
         <v>30.4</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C20" s="2">
+      <c r="AB20" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C21" s="2">
         <v>3.5</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D21" s="2">
         <v>3.5</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E21" s="2">
         <v>2.5</v>
       </c>
-      <c r="F20" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="G20" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H20" s="2">
+      <c r="F21" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="H21" s="2">
         <v>8.2</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I21" s="2">
         <v>9.0</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J21" s="2">
         <v>21.0</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K21" s="2">
         <v>21.0</v>
       </c>
-      <c r="L20" s="2">
+      <c r="L21" s="2">
         <v>6.0</v>
       </c>
-      <c r="M20" s="2">
+      <c r="M21" s="2">
         <v>1.5</v>
       </c>
-      <c r="N20" s="2">
+      <c r="N21" s="2">
         <v>1.6</v>
       </c>
-      <c r="O20" s="2">
+      <c r="O21" s="2">
         <v>2.9</v>
       </c>
-      <c r="P20" s="2">
+      <c r="P21" s="2">
         <v>4.0</v>
       </c>
-      <c r="Q20" s="2">
+      <c r="Q21" s="2">
         <v>7.3</v>
       </c>
-      <c r="R20" s="2">
+      <c r="R21" s="2">
         <v>7.8</v>
       </c>
-      <c r="S20" s="2">
+      <c r="S21" s="2">
         <v>9.7</v>
       </c>
-      <c r="T20" s="2">
+      <c r="T21" s="2">
         <v>7.5</v>
       </c>
-      <c r="U20" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="V20" s="2">
+      <c r="U21" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="V21" s="2">
         <v>70.0</v>
       </c>
-      <c r="W20" s="3">
+      <c r="W21" s="2">
         <v>80.0</v>
       </c>
-      <c r="X20" s="2">
+      <c r="X21" s="2">
         <v>70.0</v>
       </c>
-      <c r="Y20" s="3">
+      <c r="Y21" s="2">
         <v>100.0</v>
       </c>
-      <c r="Z20" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="AA20" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C21" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E21" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F21" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="G21" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H21" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="I21" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="J21" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="K21" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="L21" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="M21" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="N21" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="O21" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="P21" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="Q21" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="R21" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="S21" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="T21" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="U21" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="V21" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="W21" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="X21" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="Y21" s="2">
-        <v>0.0</v>
-      </c>
       <c r="Z21" s="2">
         <v>0.0</v>
       </c>
       <c r="AA21" s="2">
         <v>0.0</v>
       </c>
+      <c r="AB21" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" s="6" t="s">
-        <v>50</v>
+      <c r="A22" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="B22" s="2">
         <v>0.0</v>
@@ -2439,97 +2518,103 @@
       <c r="AA22" s="2">
         <v>0.0</v>
       </c>
+      <c r="AB22" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" s="6" t="s">
-        <v>51</v>
+      <c r="A23" s="7" t="s">
+        <v>54</v>
       </c>
       <c r="B23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="N23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="O23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="P23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="R23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="S23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="U23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="V23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="W23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="X23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Y23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Z23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AA23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AB23" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="2">
         <v>71.0</v>
       </c>
-      <c r="C23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="G23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="I23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="J23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="K23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="L23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="M23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="N23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="O23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="P23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="Q23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="R23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="S23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="T23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="U23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="V23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="W23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="X23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="Y23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="Z23" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="AA23" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="2">
-        <v>0.0</v>
-      </c>
       <c r="C24" s="2">
         <v>0.0</v>
       </c>
@@ -2579,92 +2664,95 @@
         <v>0.0</v>
       </c>
       <c r="S24" s="2">
-        <f>0.6*SUM(S18:S20)</f>
+        <v>0.0</v>
+      </c>
+      <c r="T24" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="U24" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="V24" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="W24" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="X24" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Y24" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Z24" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AA24" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AB24" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="I25" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="J25" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K25" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="L25" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M25" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="N25" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="O25" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="P25" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="R25" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="S25" s="2">
+        <f>0.6*SUM(S19:S21)</f>
         <v>13.8</v>
       </c>
-      <c r="T24" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="U24" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="V24" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="W24" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="X24" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="Y24" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="Z24" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="AA24" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C25" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E25" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F25" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="G25" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H25" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="I25" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="J25" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="K25" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="L25" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="M25" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="N25" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="O25" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="P25" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="Q25" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="R25" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="S25" s="2">
-        <v>0.0</v>
-      </c>
       <c r="T25" s="2">
         <v>0.0</v>
       </c>
@@ -2689,10 +2777,13 @@
       <c r="AA25" s="2">
         <v>0.0</v>
       </c>
+      <c r="AB25" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" s="6" t="s">
-        <v>54</v>
+      <c r="A26" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="B26" s="2">
         <v>0.0</v>
@@ -2772,10 +2863,13 @@
       <c r="AA26" s="2">
         <v>0.0</v>
       </c>
+      <c r="AB26" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" s="6" t="s">
-        <v>55</v>
+      <c r="A27" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="B27" s="2">
         <v>0.0</v>
@@ -2855,10 +2949,13 @@
       <c r="AA27" s="2">
         <v>0.0</v>
       </c>
+      <c r="AB27" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" s="6" t="s">
-        <v>56</v>
+      <c r="A28" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="B28" s="2">
         <v>0.0</v>
@@ -2938,10 +3035,13 @@
       <c r="AA28" s="2">
         <v>0.0</v>
       </c>
+      <c r="AB28" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" s="6" t="s">
-        <v>57</v>
+      <c r="A29" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="B29" s="2">
         <v>0.0</v>
@@ -3000,92 +3100,95 @@
       <c r="T29" s="2">
         <v>0.0</v>
       </c>
-      <c r="U29" s="3">
+      <c r="U29" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="V29" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="W29" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="X29" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Y29" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Z29" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AA29" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AB29" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="H30" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="I30" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="J30" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K30" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="L30" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M30" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="N30" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="O30" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="P30" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Q30" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="R30" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="S30" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T30" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="U30" s="2">
         <v>20.0</v>
       </c>
-      <c r="V29" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="W29" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="X29" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="Y29" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="Z29" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="AA29" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B30" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C30" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D30" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E30" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F30" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="G30" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H30" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="I30" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="J30" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="K30" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="L30" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="M30" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="N30" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="O30" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="P30" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="Q30" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="R30" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="S30" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="T30" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="U30" s="2">
-        <v>0.0</v>
-      </c>
       <c r="V30" s="2">
         <v>0.0</v>
       </c>
@@ -3104,163 +3207,253 @@
       <c r="AA30" s="2">
         <v>0.0</v>
       </c>
+      <c r="AB30" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="M31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="N31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="O31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="P31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="R31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="S31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="T31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="U31" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="V31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="W31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="X31" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA31" s="2" t="s">
-        <v>61</v>
+      <c r="A31" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="I31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="J31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="L31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="N31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="O31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="P31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Q31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="R31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="S31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="U31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="V31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="W31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="X31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Y31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Z31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AA31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AB31" s="2">
+        <v>0.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="U32" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="X32" s="2">
-        <v>0.0</v>
+        <v>63</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="R32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="S32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="T32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="U32" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="V32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="W32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="X32" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB32" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B33" s="2">
-        <v>0.25</v>
+        <v>0.0</v>
       </c>
       <c r="U33" s="2">
-        <v>0.05</v>
+        <v>0.0</v>
       </c>
       <c r="X33" s="2">
-        <v>0.18</v>
+        <v>0.0</v>
+      </c>
+      <c r="AB33" s="2">
+        <v>0.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B34" s="2">
-        <v>2.1</v>
+        <v>0.25</v>
       </c>
       <c r="U34" s="2">
-        <v>1.5</v>
+        <v>0.05</v>
       </c>
       <c r="X34" s="2">
-        <v>2.0</v>
+        <v>0.18</v>
+      </c>
+      <c r="AB34" s="2">
+        <v>0.5</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B35" s="2">
-        <v>0.23</v>
+        <v>2.1</v>
       </c>
       <c r="U35" s="2">
-        <v>0.0</v>
+        <v>1.5</v>
       </c>
       <c r="X35" s="2">
-        <v>0.3</v>
+        <v>2.0</v>
+      </c>
+      <c r="AB35" s="2">
+        <v>2.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B36" s="2">
-        <v>0.0</v>
+        <v>0.23</v>
       </c>
       <c r="U36" s="2">
         <v>0.0</v>
       </c>
       <c r="X36" s="2">
-        <v>0.0</v>
+        <v>0.3</v>
+      </c>
+      <c r="AB36" s="2">
+        <v>0.05</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B37" s="2">
         <v>0.0</v>
@@ -3269,12 +3462,15 @@
         <v>0.0</v>
       </c>
       <c r="X37" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AB37" s="2">
         <v>0.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B38" s="2">
         <v>0.0</v>
@@ -3283,12 +3479,15 @@
         <v>0.0</v>
       </c>
       <c r="X38" s="2">
-        <v>20.0</v>
+        <v>0.0</v>
+      </c>
+      <c r="AB38" s="2">
+        <v>0.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B39" s="2">
         <v>0.0</v>
@@ -3297,68 +3496,83 @@
         <v>0.0</v>
       </c>
       <c r="X39" s="2">
+        <v>20.0</v>
+      </c>
+      <c r="AB39" s="2">
         <v>0.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B40" s="2">
-        <v>87.0</v>
+        <v>0.0</v>
       </c>
       <c r="U40" s="2">
         <v>0.0</v>
       </c>
       <c r="X40" s="2">
         <v>0.0</v>
+      </c>
+      <c r="AB40" s="2">
+        <v>10.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B41" s="2">
-        <v>0.0</v>
+        <v>87.0</v>
       </c>
       <c r="U41" s="2">
         <v>0.0</v>
       </c>
       <c r="X41" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AB41" s="2">
         <v>0.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B42" s="2">
         <v>0.0</v>
       </c>
       <c r="U42" s="2">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="X42" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AB42" s="2">
         <v>0.0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B43" s="2">
         <v>0.0</v>
       </c>
       <c r="U43" s="2">
-        <v>0.0</v>
+        <v>100.0</v>
       </c>
       <c r="X43" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AB43" s="2">
         <v>0.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B44" s="2">
         <v>0.0</v>
@@ -3367,12 +3581,15 @@
         <v>0.0</v>
       </c>
       <c r="X44" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AB44" s="2">
         <v>0.0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B45" s="2">
         <v>0.0</v>
@@ -3381,12 +3598,15 @@
         <v>0.0</v>
       </c>
       <c r="X45" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AB45" s="2">
         <v>0.0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B46" s="2">
         <v>0.0</v>
@@ -3395,12 +3615,15 @@
         <v>0.0</v>
       </c>
       <c r="X46" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AB46" s="2">
         <v>0.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B47" s="2">
         <v>0.0</v>
@@ -3409,12 +3632,15 @@
         <v>0.0</v>
       </c>
       <c r="X47" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AB47" s="2">
         <v>0.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B48" s="2">
         <v>0.0</v>
@@ -3425,173 +3651,247 @@
       <c r="X48" s="2">
         <v>0.0</v>
       </c>
+      <c r="AB48" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="49">
-      <c r="A49" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="K49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="L49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="M49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="N49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="O49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="P49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="R49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="S49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="T49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="U49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="V49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="W49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="X49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA49" s="2" t="s">
-        <v>61</v>
+      <c r="A49" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B49" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="U49" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="X49" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AB49" s="2">
+        <v>0.0</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="6" t="s">
-        <v>80</v>
+      <c r="A50" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="O50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="P50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="R50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="S50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="T50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="U50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="V50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="W50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="X50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB50" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="6" t="s">
-        <v>81</v>
+      <c r="A51" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB51" s="2">
+        <v>1.3</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="6" t="s">
-        <v>82</v>
+      <c r="A52" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB52" s="2">
+        <v>0.5</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="6" t="s">
-        <v>83</v>
+      <c r="A53" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB53" s="2">
+        <v>2.0</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="6" t="s">
-        <v>84</v>
+      <c r="A54" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB54" s="2">
+        <v>0.05</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="6" t="s">
-        <v>85</v>
+      <c r="A55" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB55" s="2">
+        <v>0.0</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="6" t="s">
-        <v>86</v>
+      <c r="A56" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB56" s="2">
+        <v>0.0</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="6" t="s">
-        <v>87</v>
+      <c r="A57" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB57" s="2">
+        <v>0.0</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="6" t="s">
-        <v>88</v>
+      <c r="A58" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB58" s="2">
+        <v>0.0</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="6" t="s">
-        <v>89</v>
+      <c r="A59" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB59" s="2">
+        <v>0.0</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="6" t="s">
-        <v>90</v>
+      <c r="A60" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB60" s="2">
+        <v>0.0</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="6" t="s">
-        <v>91</v>
+      <c r="A61" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB61" s="2">
+        <v>0.0</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="6" t="s">
-        <v>92</v>
+      <c r="A62" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="AB62" s="2">
+        <v>660.0</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="6" t="s">
-        <v>93</v>
+      <c r="A63" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB63" s="2">
+        <v>0.0</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="6" t="s">
-        <v>94</v>
+      <c r="A64" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB64" s="2">
+        <v>0.0</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="6" t="s">
-        <v>95</v>
+      <c r="A65" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB65" s="2">
+        <v>0.0</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="6" t="s">
-        <v>96</v>
+      <c r="A66" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB66" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB67" s="2">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>